<commit_message>
canConstruct DP problem solving
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -150,9 +150,6 @@
     <t>https://leetcode.com/problems/longest-palindromic-substring/</t>
   </si>
   <si>
-    <t>Longest Palindrome Substring</t>
-  </si>
-  <si>
     <t>https://leetcode.com/problems/running-sum-of-1d-array/</t>
   </si>
   <si>
@@ -421,6 +418,33 @@
   </si>
   <si>
     <t>Minimum Operations to Reduce X to Zero (June Day-11)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/word-break/</t>
+  </si>
+  <si>
+    <t>42. String + DP</t>
+  </si>
+  <si>
+    <t>Word Break</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-cameras/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/prefix-and-suffix-search/</t>
+  </si>
+  <si>
+    <t>Binary Tree Cameras (June Day-17)</t>
+  </si>
+  <si>
+    <t>Prefix and Suffix Search (June Day-18)</t>
+  </si>
+  <si>
+    <t>Longest Palindrome Substring (June Day-16)</t>
+  </si>
+  <si>
+    <t>43. Tree</t>
   </si>
 </sst>
 </file>
@@ -607,7 +631,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -636,6 +660,7 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -946,7 +971,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -954,9 +979,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
@@ -1077,7 +1102,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
@@ -1116,7 +1141,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>33</v>
@@ -1127,13 +1152,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>36</v>
@@ -1141,7 +1166,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>37</v>
@@ -1152,7 +1177,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>16</v>
@@ -1163,10 +1188,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>42</v>
@@ -1174,303 +1199,336 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="D18" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>59</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>70</v>
-      </c>
       <c r="D23" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29" t="s">
-        <v>92</v>
-      </c>
       <c r="D29" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>95</v>
-      </c>
       <c r="D30" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="D31" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>103</v>
-      </c>
       <c r="D32" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" t="s">
         <v>116</v>
       </c>
-      <c r="B37" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" t="s">
-        <v>117</v>
-      </c>
       <c r="D37" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C39" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C39" t="s">
-        <v>122</v>
-      </c>
       <c r="D39" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>129</v>
-      </c>
       <c r="C41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1514,8 +1572,11 @@
     <hyperlink ref="D39" r:id="rId37"/>
     <hyperlink ref="D40" r:id="rId38"/>
     <hyperlink ref="D41" r:id="rId39"/>
+    <hyperlink ref="D42" r:id="rId40"/>
+    <hyperlink ref="D43" r:id="rId41"/>
+    <hyperlink ref="D44" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId43"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved some more DP questions
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="147">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -445,6 +445,21 @@
   </si>
   <si>
     <t>43. Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/combination-sum-iv/</t>
+  </si>
+  <si>
+    <t>Combination Sum IV</t>
+  </si>
+  <si>
+    <t>45. Array + DP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/search-suggestions-system/</t>
+  </si>
+  <si>
+    <t>Search Suggestions System (June Day-19)</t>
   </si>
 </sst>
 </file>
@@ -971,7 +986,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -979,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,14 +1536,30 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>44</v>
-      </c>
       <c r="B44" s="16" t="s">
         <v>139</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1575,8 +1606,10 @@
     <hyperlink ref="D42" r:id="rId40"/>
     <hyperlink ref="D43" r:id="rId41"/>
     <hyperlink ref="D44" r:id="rId42"/>
+    <hyperlink ref="D45" r:id="rId43"/>
+    <hyperlink ref="D46" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId43"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-20 for June Challenge
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="152">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -460,6 +460,21 @@
   </si>
   <si>
     <t>Search Suggestions System (June Day-19)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/short-encoding-of-words/</t>
+  </si>
+  <si>
+    <t>Short Encoding of Words (June Day-20)</t>
+  </si>
+  <si>
+    <t>47. String</t>
+  </si>
+  <si>
+    <t>Use std::set</t>
+  </si>
+  <si>
+    <t>46. Trie</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1001,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -994,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,11 +1570,28 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>151</v>
+      </c>
       <c r="B46" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" t="s">
+        <v>150</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1608,8 +1640,9 @@
     <hyperlink ref="D44" r:id="rId42"/>
     <hyperlink ref="D45" r:id="rId43"/>
     <hyperlink ref="D46" r:id="rId44"/>
+    <hyperlink ref="D47" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId45"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation of Trie Data Structure
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="156">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -474,7 +474,19 @@
     <t>Use std::set</t>
   </si>
   <si>
-    <t>46. Trie</t>
+    <t>https://leetcode.com/problems/implement-trie-prefix-tree/</t>
+  </si>
+  <si>
+    <t>Implement Trie (Prefix Tree)</t>
+  </si>
+  <si>
+    <t>48. Trie DS</t>
+  </si>
+  <si>
+    <t>46. Trie DS</t>
+  </si>
+  <si>
+    <t>But I can use hashmap instead of trie data structure</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1009,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,10 +1583,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>146</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>145</v>
@@ -1592,6 +1607,17 @@
       </c>
       <c r="D47" s="9" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1641,8 +1667,9 @@
     <hyperlink ref="D45" r:id="rId43"/>
     <hyperlink ref="D46" r:id="rId44"/>
     <hyperlink ref="D47" r:id="rId45"/>
+    <hyperlink ref="D48" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-21 for June Challenge
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -487,6 +487,15 @@
   </si>
   <si>
     <t>But I can use hashmap instead of trie data structure</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/furthest-building-you-can-reach/</t>
+  </si>
+  <si>
+    <t>Furthest Building You Can Reach (June Day-21)</t>
+  </si>
+  <si>
+    <t>49. Priority Queue</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1022,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1021,10 +1030,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,6 +1627,17 @@
       </c>
       <c r="D48" s="9" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1668,8 +1688,9 @@
     <hyperlink ref="D46" r:id="rId44"/>
     <hyperlink ref="D47" r:id="rId45"/>
     <hyperlink ref="D48" r:id="rId46"/>
+    <hyperlink ref="D49" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-22 for June Challenge
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -495,7 +495,19 @@
     <t>Furthest Building You Can Reach (June Day-21)</t>
   </si>
   <si>
-    <t>49. Priority Queue</t>
+    <t>https://leetcode.com/problems/kth-largest-element-in-an-array/</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>50. Priority Queue + Heap</t>
+  </si>
+  <si>
+    <t>49. Priority Queue + Heap</t>
+  </si>
+  <si>
+    <t>Use min heap to solve this problem</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1034,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1030,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1631,13 +1643,27 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>157</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>160</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1689,8 +1715,9 @@
     <hyperlink ref="D47" r:id="rId45"/>
     <hyperlink ref="D48" r:id="rId46"/>
     <hyperlink ref="D49" r:id="rId47"/>
+    <hyperlink ref="D50" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId48"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-24 for June Challenge
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="169">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -498,9 +498,6 @@
     <t>https://leetcode.com/problems/kth-largest-element-in-an-array/</t>
   </si>
   <si>
-    <t>Kth Largest Element in an Array</t>
-  </si>
-  <si>
     <t>50. Priority Queue + Heap</t>
   </si>
   <si>
@@ -508,6 +505,27 @@
   </si>
   <si>
     <t>Use min heap to solve this problem</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/course-schedule-iii/</t>
+  </si>
+  <si>
+    <t>51. Graph</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array (June Day-22)</t>
+  </si>
+  <si>
+    <t>Course Schedule III (June Day-23)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/construct-target-array-with-multiple-sums/</t>
+  </si>
+  <si>
+    <t>52. Arrays + Heap</t>
+  </si>
+  <si>
+    <t>Construct Target Array With Multiple Sums (June Day-24)</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1052,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1042,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1661,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>157</v>
@@ -1654,16 +1672,38 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>163</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>167</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1716,8 +1756,10 @@
     <hyperlink ref="D48" r:id="rId46"/>
     <hyperlink ref="D49" r:id="rId47"/>
     <hyperlink ref="D50" r:id="rId48"/>
+    <hyperlink ref="D51" r:id="rId49"/>
+    <hyperlink ref="D52" r:id="rId50"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId49"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day-26 for June Challenge
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="175">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -526,6 +526,24 @@
   </si>
   <si>
     <t>Construct Target Array With Multiple Sums (June Day-24)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/non-decreasing-array/</t>
+  </si>
+  <si>
+    <t>53. Arrays</t>
+  </si>
+  <si>
+    <t>Non-decreasing Array (June Day-25)</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-points-you-can-obtain-from-cards/</t>
+  </si>
+  <si>
+    <t>Maximum Points You Can Obtain from Cards (June Day-26)</t>
+  </si>
+  <si>
+    <t>54. Sliding Window</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1070,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1060,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,6 +1722,28 @@
       </c>
       <c r="D52" s="9" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1758,8 +1798,10 @@
     <hyperlink ref="D50" r:id="rId48"/>
     <hyperlink ref="D51" r:id="rId49"/>
     <hyperlink ref="D52" r:id="rId50"/>
+    <hyperlink ref="D53" r:id="rId51"/>
+    <hyperlink ref="D54" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId53"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
completed june leetcoding challenge
</commit_message>
<xml_diff>
--- a/My LeetCode.xlsx
+++ b/My LeetCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="187">
   <si>
     <t>LeetCode Problems</t>
   </si>
@@ -544,6 +544,42 @@
   </si>
   <si>
     <t>54. Sliding Window</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-moves-to-equal-array-elements-ii/</t>
+  </si>
+  <si>
+    <t>Minimum Moves to Equal Array Elements II</t>
+  </si>
+  <si>
+    <t>55. Arrays</t>
+  </si>
+  <si>
+    <t>Queue Reconstruction by Height</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/queue-reconstruction-by-height/</t>
+  </si>
+  <si>
+    <t>56. Queue</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-deletions-to-make-character-frequencies-unique/</t>
+  </si>
+  <si>
+    <t>Minimum Deletions to Make Character Frequencies Unique</t>
+  </si>
+  <si>
+    <t>57. Strings</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/partitioning-into-minimum-number-of-deci-binary-numbers/</t>
+  </si>
+  <si>
+    <t>Partitioning Into Minimum Number Of Deci-Binary Numbers</t>
+  </si>
+  <si>
+    <t>58. Numbers</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1106,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1078,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,6 +1780,50 @@
       </c>
       <c r="D54" s="9" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>177</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>180</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1800,8 +1880,12 @@
     <hyperlink ref="D52" r:id="rId50"/>
     <hyperlink ref="D53" r:id="rId51"/>
     <hyperlink ref="D54" r:id="rId52"/>
+    <hyperlink ref="D55" r:id="rId53"/>
+    <hyperlink ref="D56" r:id="rId54"/>
+    <hyperlink ref="D57" r:id="rId55"/>
+    <hyperlink ref="D58" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId53"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>